<commit_message>
Changes added - Excel sheet added
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Admin</t>
   </si>
@@ -43,6 +37,9 @@
   </si>
   <si>
     <t>Admin1234</t>
+  </si>
+  <si>
+    <t>Paswword123</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -391,39 +388,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Changes added - Excel sheet added"
This reverts commit b53075e73861814130a23d4b065d2355ee84023f.
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -16,7 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
   <si>
     <t>Admin</t>
   </si>
@@ -37,9 +43,6 @@
   </si>
   <si>
     <t>Admin1234</t>
-  </si>
-  <si>
-    <t>Paswword123</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -388,39 +391,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new test case
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Admin</t>
   </si>
@@ -43,6 +37,9 @@
   </si>
   <si>
     <t>Admin1234</t>
+  </si>
+  <si>
+    <t>Paswword123</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -391,39 +388,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>